<commit_message>
changed input format to include the summation of sep and reatt bars volumes and areas
</commit_message>
<xml_diff>
--- a/LU_Max_Vol.xlsx
+++ b/LU_Max_Vol.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1276,14 +1276,14 @@
   <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+      <selection activeCell="C57" sqref="C57:F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="5" width="22.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="2" max="5" width="22.125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="30.75" customWidth="1"/>
+    <col min="7" max="7" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1507,9 +1507,22 @@
       <c r="B12" s="9">
         <v>64178.180834873201</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
+      <c r="C12" s="4">
+        <f>C13+C14</f>
+        <v>61639.484819255602</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" ref="D12:F12" si="0">D13+D14</f>
+        <v>4236.7940711061401</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>474.18408276825994</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>21059</v>
+      </c>
       <c r="G12" s="10">
         <v>22323</v>
       </c>
@@ -1557,10 +1570,22 @@
       <c r="B15" s="9">
         <v>15395.537510042283</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
+      <c r="C15" s="9">
+        <f>C16+C17</f>
+        <v>47224.5043115882</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" ref="D15:F15" si="1">D16+D17</f>
+        <v>19160.722828614988</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" si="1"/>
+        <v>5809.96963154681</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="1"/>
+        <v>40328</v>
+      </c>
       <c r="G15" s="10">
         <v>18125</v>
       </c>
@@ -1630,10 +1655,22 @@
       <c r="B19" s="9">
         <v>36182.601113095501</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
+      <c r="C19" s="9">
+        <f>C20+C21</f>
+        <v>59402.16337770359</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" ref="D19:F19" si="2">D20+D21</f>
+        <v>12686.043215566613</v>
+      </c>
+      <c r="E19" s="9">
+        <f t="shared" si="2"/>
+        <v>4357.8450600947872</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="2"/>
+        <v>25428</v>
+      </c>
       <c r="G19" s="10">
         <v>18585</v>
       </c>
@@ -1680,10 +1717,22 @@
       <c r="B22" s="9">
         <v>8362.4010828012106</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
+      <c r="C22" s="9">
+        <f>C23+C24</f>
+        <v>35761.109003689598</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" ref="D22" si="3">D23+D24</f>
+        <v>9544.2709237140589</v>
+      </c>
+      <c r="E22" s="9">
+        <f t="shared" ref="E22" si="4">E23+E24</f>
+        <v>2427.6204097683399</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" ref="F22" si="5">F23+F24</f>
+        <v>22540</v>
+      </c>
       <c r="G22" s="10">
         <v>13279</v>
       </c>
@@ -1758,10 +1807,22 @@
       <c r="B26" s="9">
         <v>15120.918770161999</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="10"/>
+      <c r="C26" s="9">
+        <f>C27+C28</f>
+        <v>7458.1155740411996</v>
+      </c>
+      <c r="D26" s="9">
+        <f t="shared" ref="D26" si="6">D27+D28</f>
+        <v>4860.7447832371709</v>
+      </c>
+      <c r="E26" s="9">
+        <f t="shared" ref="E26" si="7">E27+E28</f>
+        <v>3179.5580318836301</v>
+      </c>
+      <c r="F26" s="9">
+        <f t="shared" ref="F26" si="8">F27+F28</f>
+        <v>9147</v>
+      </c>
       <c r="G26" s="10">
         <v>10484</v>
       </c>
@@ -1893,10 +1954,22 @@
       <c r="B33" s="9">
         <v>95132.002700075856</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10"/>
+      <c r="C33" s="9">
+        <f>C34+C35</f>
+        <v>119011.06450036528</v>
+      </c>
+      <c r="D33" s="9">
+        <f t="shared" ref="D33:F33" si="9">D34+D35</f>
+        <v>16023.351264585786</v>
+      </c>
+      <c r="E33" s="9">
+        <f t="shared" si="9"/>
+        <v>5356.2145517119197</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" si="9"/>
+        <v>27853</v>
+      </c>
       <c r="G33" s="10">
         <v>27448</v>
       </c>
@@ -1943,10 +2016,22 @@
       <c r="B36" s="9">
         <v>52927.691167440382</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="10"/>
+      <c r="C36" s="9">
+        <f>C37+C38</f>
+        <v>39431.970142152037</v>
+      </c>
+      <c r="D36" s="9">
+        <f t="shared" ref="D36:F36" si="10">D37+D38</f>
+        <v>11297.952868331848</v>
+      </c>
+      <c r="E36" s="9">
+        <f t="shared" si="10"/>
+        <v>2798.96919226011</v>
+      </c>
+      <c r="F36" s="9">
+        <f t="shared" si="10"/>
+        <v>16220</v>
+      </c>
       <c r="G36" s="10">
         <v>19812</v>
       </c>
@@ -2380,10 +2465,22 @@
       <c r="B57" s="9">
         <v>16670.720221737007</v>
       </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="10"/>
+      <c r="C57" s="9">
+        <f>C58+C59</f>
+        <v>43214.982671747581</v>
+      </c>
+      <c r="D57" s="9">
+        <f t="shared" ref="D57:F57" si="11">D58+D59</f>
+        <v>3565.6722644960801</v>
+      </c>
+      <c r="E57" s="9">
+        <f t="shared" si="11"/>
+        <v>1323.7435055953301</v>
+      </c>
+      <c r="F57" s="9">
+        <f t="shared" si="11"/>
+        <v>13937</v>
+      </c>
       <c r="G57" s="10">
         <v>7084</v>
       </c>

</xml_diff>